<commit_message>
fix excel file and fix path
</commit_message>
<xml_diff>
--- a/CovidForm/oprosnik.xlsx
+++ b/CovidForm/oprosnik.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9730A4E2-E364-41D6-B8DC-875A7505A705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E57F3FA-6970-43A2-924C-F8F294599AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3990" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Опросник" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,10 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="Гам_КОВИД_Вак">Опросник!$BS$71:$BS$73</definedName>
+    <definedName name="Гам_КОВИД_Вак">Опросник!$BR$71:$BR$73</definedName>
     <definedName name="кашель_влажный">В одну [1]ячейку!$B$54</definedName>
-    <definedName name="корона">Опросник!$BS$71:$BS$73</definedName>
-    <definedName name="список">Опросник!$BS$71:$BS$73</definedName>
+    <definedName name="корона">Опросник!$BR$71:$BR$73</definedName>
+    <definedName name="список">Опросник!$BR$71:$BR$73</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1240,7 +1240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1539,6 +1539,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1552,19 +1561,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1998,8 +1995,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица10" displayName="Таблица10" ref="BS1:BS25" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
-  <autoFilter ref="BS1:BS25" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица10" displayName="Таблица10" ref="BR1:BR25" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
+  <autoFilter ref="BR1:BR25" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Группа лиц" dataDxfId="13"/>
   </tableColumns>
@@ -2418,30 +2415,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BS103"/>
+  <dimension ref="A1:BR103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="118"/>
-    <col min="2" max="2" width="59.42578125" style="38" customWidth="1"/>
-    <col min="3" max="3" width="58.5703125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="71" max="71" width="48.7109375" style="45" customWidth="1"/>
+    <col min="1" max="1" width="59.42578125" style="38" customWidth="1"/>
+    <col min="2" max="2" width="58.5703125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="70" max="70" width="48.7109375" style="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="106" t="s">
+    <row r="1" spans="1:70" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="106" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="107"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -2455,1149 +2452,851 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="BS1" s="42" t="s">
+      <c r="R1" s="2"/>
+      <c r="BR1" s="42" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:71" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="108" t="s">
+    <row r="2" spans="1:70" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="109"/>
-      <c r="D2" s="1"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="BS2" s="43" t="s">
+      <c r="BR2" s="43" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:71" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="118">
+    <row r="3" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="99" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="54"/>
+      <c r="B3" s="54"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="BS3" s="44" t="s">
+      <c r="BR3" s="44" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:71" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="118">
-        <v>2</v>
-      </c>
-      <c r="B4" s="100" t="s">
+    <row r="4" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="100" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="BS4" s="43" t="s">
+      <c r="BR4" s="43" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:71" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="118">
-        <v>3</v>
-      </c>
-      <c r="B5" s="100" t="s">
+    <row r="5" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="BS5" s="44" t="s">
+      <c r="BR5" s="44" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:71" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="118">
-        <v>4</v>
-      </c>
-      <c r="B6" s="100" t="s">
+    <row r="6" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="BS6" s="43" t="s">
+      <c r="BR6" s="43" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:71" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="118">
-        <v>5</v>
-      </c>
-      <c r="B7" s="100" t="s">
+    <row r="7" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="BS7" s="44" t="s">
+      <c r="BR7" s="44" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:71" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="118">
-        <v>6</v>
-      </c>
-      <c r="B8" s="100" t="s">
+    <row r="8" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="100" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="BS8" s="43" t="s">
+      <c r="BR8" s="43" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:71" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="118">
+    <row r="9" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="100" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="BS9" s="44" t="s">
+      <c r="BR9" s="44" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:71" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="118">
-        <v>8</v>
-      </c>
-      <c r="B10" s="100" t="s">
+    <row r="10" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="100" t="s">
         <v>130</v>
       </c>
-      <c r="C10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="BS10" s="43" t="s">
+      <c r="BR10" s="43" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:71" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="118">
-        <v>9</v>
-      </c>
-      <c r="B11" s="100" t="s">
+    <row r="11" spans="1:70" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="BS11" s="44" t="s">
+      <c r="BR11" s="44" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:71" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="118">
-        <v>10</v>
-      </c>
-      <c r="B12" s="100" t="s">
+    <row r="12" spans="1:70" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="4"/>
-      <c r="BS12" s="43" t="s">
+      <c r="B12" s="24"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="4"/>
+      <c r="BR12" s="43" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:71" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="118">
-        <v>11</v>
-      </c>
-      <c r="B13" s="100" t="s">
+    <row r="13" spans="1:70" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="C13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="BS13" s="44" t="s">
+      <c r="BR13" s="44" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="118">
-        <v>12</v>
-      </c>
-      <c r="B14" s="100" t="s">
+    <row r="14" spans="1:70" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="100" t="s">
         <v>133</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="BS14" s="43" t="s">
+      <c r="BR14" s="43" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:71" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="118">
-        <v>13</v>
-      </c>
-      <c r="B15" s="100" t="s">
+    <row r="15" spans="1:70" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="100" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="BS15" s="44" t="s">
+      <c r="BR15" s="44" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:71" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="118">
-        <v>14</v>
-      </c>
-      <c r="B16" s="100" t="s">
+    <row r="16" spans="1:70" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="100" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="BS16" s="43" t="s">
+      <c r="BR16" s="43" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="17" spans="1:71" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="118">
-        <v>15</v>
-      </c>
-      <c r="B17" s="101" t="s">
+    <row r="17" spans="1:70" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="101" t="s">
         <v>160</v>
       </c>
-      <c r="C17" s="55"/>
+      <c r="B17" s="55"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="BS17" s="51"/>
-    </row>
-    <row r="18" spans="1:71" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="118">
-        <v>16</v>
-      </c>
-      <c r="B18" s="101" t="s">
+      <c r="BR17" s="51"/>
+    </row>
+    <row r="18" spans="1:70" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="55"/>
+      <c r="B18" s="55"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="BS18" s="51"/>
-    </row>
-    <row r="19" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="118">
-        <v>17</v>
-      </c>
-      <c r="B19" s="100" t="s">
+      <c r="BR18" s="51"/>
+    </row>
+    <row r="19" spans="1:70" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="100" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="BS19" s="44" t="s">
+      <c r="BR19" s="44" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="118">
-        <v>18</v>
-      </c>
-      <c r="B20" s="101" t="s">
+    <row r="20" spans="1:70" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="55"/>
+      <c r="B20" s="55"/>
+      <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="BS20" s="52"/>
-    </row>
-    <row r="21" spans="1:71" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="118">
-        <v>19</v>
-      </c>
-      <c r="B21" s="100" t="s">
+      <c r="BR20" s="52"/>
+    </row>
+    <row r="21" spans="1:70" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="C21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="BS21" s="43" t="s">
+      <c r="BR21" s="43" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="118">
-        <v>20</v>
-      </c>
-      <c r="B22" s="100" t="s">
+    <row r="22" spans="1:70" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="100" t="s">
         <v>134</v>
       </c>
-      <c r="C22" s="86"/>
-      <c r="D22" s="15"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="BS22" s="44" t="s">
+      <c r="BR22" s="44" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:71" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="118">
-        <v>21</v>
-      </c>
-      <c r="B23" s="100" t="s">
+    <row r="23" spans="1:70" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="100" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="74"/>
+      <c r="B23" s="74"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="BS23" s="43" t="s">
+      <c r="BR23" s="43" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="24" spans="1:71" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="118">
-        <v>22</v>
-      </c>
-      <c r="B24" s="100" t="s">
+    <row r="24" spans="1:70" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="100" t="s">
         <v>190</v>
       </c>
-      <c r="C24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="BS24" s="51"/>
-    </row>
-    <row r="25" spans="1:71" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="118">
-        <v>23</v>
-      </c>
-      <c r="B25" s="100" t="s">
+      <c r="BR24" s="51"/>
+    </row>
+    <row r="25" spans="1:70" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="76"/>
+      <c r="B25" s="76"/>
+      <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="BS25" s="44" t="s">
+      <c r="BR25" s="44" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:71" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="118">
-        <v>24</v>
-      </c>
-      <c r="B26" s="21" t="s">
+    <row r="26" spans="1:70" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="76"/>
+      <c r="B26" s="76"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-    </row>
-    <row r="27" spans="1:71" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="118">
-        <v>25</v>
-      </c>
-      <c r="B27" s="100" t="s">
+    </row>
+    <row r="27" spans="1:70" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="100" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="76"/>
+      <c r="B27" s="76"/>
+      <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-    </row>
-    <row r="28" spans="1:71" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="118">
-        <v>26</v>
-      </c>
-      <c r="B28" s="100" t="s">
+    </row>
+    <row r="28" spans="1:70" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="93"/>
+      <c r="B28" s="93"/>
+      <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-    </row>
-    <row r="29" spans="1:71" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="118">
-        <v>27</v>
-      </c>
-      <c r="B29" s="21" t="s">
+    </row>
+    <row r="29" spans="1:70" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="C29" s="76"/>
+      <c r="B29" s="76"/>
+      <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-    </row>
-    <row r="30" spans="1:71" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="23"/>
-      <c r="C30" s="77"/>
+    </row>
+    <row r="30" spans="1:70" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="23"/>
+      <c r="B30" s="77"/>
+      <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-    </row>
-    <row r="31" spans="1:71" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="118">
-        <v>28</v>
-      </c>
-      <c r="B31" s="105" t="s">
+    </row>
+    <row r="31" spans="1:70" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="56"/>
+      <c r="B31" s="56"/>
+      <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-    </row>
-    <row r="32" spans="1:71" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="118">
+    </row>
+    <row r="32" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="99" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="100" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="30"/>
+    </row>
+    <row r="34" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="100" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="30"/>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="100" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="30"/>
+    </row>
+    <row r="36" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="100" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="30"/>
+    </row>
+    <row r="37" spans="1:2" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="62"/>
+    </row>
+    <row r="38" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="48"/>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="34"/>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="24"/>
+    </row>
+    <row r="41" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="24"/>
+    </row>
+    <row r="42" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="24"/>
+    </row>
+    <row r="43" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="24"/>
+    </row>
+    <row r="44" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" s="24"/>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="30"/>
+    </row>
+    <row r="46" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="30"/>
+    </row>
+    <row r="47" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="30"/>
+    </row>
+    <row r="48" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="99" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="46" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="118">
+      <c r="B48" s="62"/>
+    </row>
+    <row r="49" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="100" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="30"/>
-    </row>
-    <row r="34" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="118">
+      <c r="B49" s="34"/>
+    </row>
+    <row r="50" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="100" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="30"/>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="118">
+      <c r="B50" s="50"/>
+    </row>
+    <row r="51" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="100" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="30"/>
-    </row>
-    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="118">
+      <c r="B51" s="50"/>
+    </row>
+    <row r="52" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="100" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="30"/>
-    </row>
-    <row r="37" spans="1:3" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="118">
+      <c r="B52" s="50"/>
+    </row>
+    <row r="53" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="61" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="62"/>
-    </row>
-    <row r="38" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="118">
+      <c r="B53" s="24"/>
+    </row>
+    <row r="54" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="48"/>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="118">
+      <c r="B54" s="33"/>
+    </row>
+    <row r="55" spans="1:6" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="34"/>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="118">
+      <c r="B55" s="62"/>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="24"/>
-    </row>
-    <row r="41" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="118">
+      <c r="B56" s="46"/>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="24"/>
-    </row>
-    <row r="42" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="118">
+      <c r="B57" s="24"/>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C42" s="24"/>
-    </row>
-    <row r="43" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="118">
+      <c r="B58" s="27"/>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="100" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="24"/>
-    </row>
-    <row r="44" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="118">
+      <c r="B59" s="55"/>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C44" s="24"/>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="118">
+      <c r="B60" s="55"/>
+    </row>
+    <row r="61" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="100" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="30"/>
-    </row>
-    <row r="46" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="118">
+      <c r="B61" s="24"/>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C46" s="30"/>
-    </row>
-    <row r="47" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="118">
+      <c r="B62" s="60"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="15"/>
+      <c r="F62" s="15"/>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C47" s="30"/>
-    </row>
-    <row r="48" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="118">
+      <c r="B63" s="24"/>
+      <c r="C63" s="16"/>
+      <c r="E63" s="15"/>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="100" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" s="62"/>
-    </row>
-    <row r="49" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="118">
+      <c r="B64" s="60"/>
+    </row>
+    <row r="65" spans="1:70" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="B49" s="102" t="s">
-        <v>30</v>
-      </c>
-      <c r="C49" s="34"/>
-    </row>
-    <row r="50" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="118">
+      <c r="B65" s="59"/>
+    </row>
+    <row r="66" spans="1:70" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="100" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50" s="50"/>
-    </row>
-    <row r="51" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="118">
+      <c r="B66" s="27"/>
+    </row>
+    <row r="67" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="100" t="s">
+        <v>104</v>
+      </c>
+      <c r="B67" s="60"/>
+    </row>
+    <row r="68" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="100" t="s">
+        <v>50</v>
+      </c>
+      <c r="B68" s="60"/>
+    </row>
+    <row r="69" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="100" t="s">
-        <v>32</v>
-      </c>
-      <c r="C51" s="50"/>
-    </row>
-    <row r="52" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="118">
+      <c r="B69" s="24"/>
+      <c r="C69" s="15"/>
+    </row>
+    <row r="70" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="B52" s="100" t="s">
-        <v>33</v>
-      </c>
-      <c r="C52" s="50"/>
-    </row>
-    <row r="53" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="118">
-        <v>50</v>
-      </c>
-      <c r="B53" s="100" t="s">
-        <v>34</v>
-      </c>
-      <c r="C53" s="24"/>
-    </row>
-    <row r="54" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="118">
+      <c r="B70" s="27"/>
+    </row>
+    <row r="71" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="100" t="s">
+        <v>184</v>
+      </c>
+      <c r="B71" s="30"/>
+      <c r="C71" s="15"/>
+      <c r="BR71" s="67" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="72" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="B72" s="27"/>
+      <c r="C72" s="15"/>
+      <c r="BR72" s="67" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="73" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="100" t="s">
+        <v>172</v>
+      </c>
+      <c r="B73" s="50"/>
+      <c r="C73" s="15"/>
+      <c r="BR73" s="67"/>
+    </row>
+    <row r="74" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="100" t="s">
+        <v>175</v>
+      </c>
+      <c r="B74" s="68"/>
+      <c r="C74" s="15"/>
+    </row>
+    <row r="75" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="100" t="s">
+        <v>173</v>
+      </c>
+      <c r="B75" s="50"/>
+      <c r="C75" s="15"/>
+    </row>
+    <row r="76" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="100" t="s">
+        <v>176</v>
+      </c>
+      <c r="B76" s="69"/>
+      <c r="C76" s="15"/>
+    </row>
+    <row r="77" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="100" t="s">
+        <v>189</v>
+      </c>
+      <c r="B77" s="30"/>
+    </row>
+    <row r="78" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="100" t="s">
+        <v>185</v>
+      </c>
+      <c r="B78" s="30"/>
+    </row>
+    <row r="79" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="100" t="s">
+        <v>183</v>
+      </c>
+      <c r="B79" s="30"/>
+    </row>
+    <row r="80" spans="1:70" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="103" t="s">
-        <v>35</v>
-      </c>
-      <c r="C54" s="33"/>
-    </row>
-    <row r="55" spans="1:7" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="118">
+      <c r="B80" s="19"/>
+      <c r="D80" s="14"/>
+    </row>
+    <row r="81" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="61" t="s">
-        <v>36</v>
-      </c>
-      <c r="C55" s="62"/>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="118">
+      <c r="B81" s="27"/>
+      <c r="D81" s="12"/>
+    </row>
+    <row r="82" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="104" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="99" t="s">
-        <v>37</v>
-      </c>
-      <c r="C56" s="46"/>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="118">
+      <c r="B82" s="47"/>
+      <c r="D82" s="12"/>
+    </row>
+    <row r="83" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="100" t="s">
-        <v>38</v>
-      </c>
-      <c r="C57" s="24"/>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="118">
+      <c r="B83" s="62"/>
+      <c r="D83" s="12"/>
+    </row>
+    <row r="84" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A84" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="100" t="s">
-        <v>39</v>
-      </c>
-      <c r="C58" s="27"/>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="118">
+      <c r="B84" s="74"/>
+      <c r="D84" s="12"/>
+    </row>
+    <row r="85" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="100" t="s">
-        <v>40</v>
-      </c>
-      <c r="C59" s="55"/>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="118">
+      <c r="B85" s="24"/>
+    </row>
+    <row r="86" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B86" s="35"/>
+      <c r="D86" s="12"/>
+    </row>
+    <row r="87" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B60" s="100" t="s">
-        <v>41</v>
-      </c>
-      <c r="C60" s="55"/>
-    </row>
-    <row r="61" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="118">
+      <c r="B87" s="35"/>
+      <c r="D87" s="12"/>
+    </row>
+    <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="100" t="s">
-        <v>42</v>
-      </c>
-      <c r="C61" s="24"/>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="118">
+      <c r="B88" s="35"/>
+      <c r="D88" s="12"/>
+    </row>
+    <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B62" s="100" t="s">
-        <v>43</v>
-      </c>
-      <c r="C62" s="60"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="15"/>
-      <c r="G62" s="15"/>
-    </row>
-    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="118">
+      <c r="B89" s="35"/>
+      <c r="D89" s="12"/>
+    </row>
+    <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B63" s="100" t="s">
-        <v>44</v>
-      </c>
-      <c r="C63" s="24"/>
-      <c r="D63" s="16"/>
-      <c r="F63" s="15"/>
-    </row>
-    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="118">
+      <c r="B90" s="35"/>
+    </row>
+    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B64" s="100" t="s">
-        <v>45</v>
-      </c>
-      <c r="C64" s="60"/>
-    </row>
-    <row r="65" spans="1:71" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="118">
+      <c r="B91" s="35"/>
+    </row>
+    <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B65" s="100" t="s">
-        <v>46</v>
-      </c>
-      <c r="C65" s="59"/>
-    </row>
-    <row r="66" spans="1:71" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="118">
+      <c r="B92" s="35"/>
+    </row>
+    <row r="93" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B66" s="100" t="s">
-        <v>47</v>
-      </c>
-      <c r="C66" s="27"/>
-    </row>
-    <row r="67" spans="1:71" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="118">
+      <c r="B93" s="35"/>
+    </row>
+    <row r="94" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B67" s="100" t="s">
-        <v>104</v>
-      </c>
-      <c r="C67" s="60"/>
-    </row>
-    <row r="68" spans="1:71" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="118">
+      <c r="B94" s="35"/>
+    </row>
+    <row r="95" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B68" s="100" t="s">
-        <v>50</v>
-      </c>
-      <c r="C68" s="60"/>
-    </row>
-    <row r="69" spans="1:71" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="118">
+      <c r="B95" s="35"/>
+    </row>
+    <row r="96" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B69" s="100" t="s">
-        <v>48</v>
-      </c>
-      <c r="C69" s="24"/>
-      <c r="D69" s="15"/>
-    </row>
-    <row r="70" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="118">
+      <c r="B96" s="95"/>
+    </row>
+    <row r="97" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B70" s="100" t="s">
-        <v>49</v>
-      </c>
-      <c r="C70" s="27"/>
-    </row>
-    <row r="71" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="118">
+      <c r="B97" s="35"/>
+    </row>
+    <row r="98" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B71" s="100" t="s">
-        <v>184</v>
-      </c>
-      <c r="C71" s="30"/>
-      <c r="D71" s="15"/>
-      <c r="BS71" s="67" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="72" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="118">
+      <c r="B98" s="35"/>
+    </row>
+    <row r="99" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A99" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="C72" s="27"/>
-      <c r="D72" s="15"/>
-      <c r="BS72" s="67" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="73" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="118">
+      <c r="B99" s="41"/>
+    </row>
+    <row r="100" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B73" s="100" t="s">
-        <v>172</v>
-      </c>
-      <c r="C73" s="50"/>
-      <c r="D73" s="15"/>
-      <c r="BS73" s="67"/>
-    </row>
-    <row r="74" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="118">
+      <c r="B100" s="41"/>
+      <c r="C100" s="15"/>
+    </row>
+    <row r="101" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A101" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B74" s="100" t="s">
-        <v>175</v>
-      </c>
-      <c r="C74" s="68"/>
-      <c r="D74" s="15"/>
-    </row>
-    <row r="75" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="118">
+      <c r="B101" s="41"/>
+      <c r="C101" s="15"/>
+    </row>
+    <row r="102" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="B75" s="100" t="s">
-        <v>173</v>
-      </c>
-      <c r="C75" s="50"/>
-      <c r="D75" s="15"/>
-    </row>
-    <row r="76" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="118">
-        <v>73</v>
-      </c>
-      <c r="B76" s="100" t="s">
-        <v>176</v>
-      </c>
-      <c r="C76" s="69"/>
-      <c r="D76" s="15"/>
-    </row>
-    <row r="77" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="118">
-        <v>74</v>
-      </c>
-      <c r="B77" s="100" t="s">
-        <v>189</v>
-      </c>
-      <c r="C77" s="30"/>
-    </row>
-    <row r="78" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="118">
-        <v>75</v>
-      </c>
-      <c r="B78" s="100" t="s">
-        <v>185</v>
-      </c>
-      <c r="C78" s="30"/>
-    </row>
-    <row r="79" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="118">
-        <v>76</v>
-      </c>
-      <c r="B79" s="100" t="s">
-        <v>183</v>
-      </c>
-      <c r="C79" s="30"/>
-    </row>
-    <row r="80" spans="1:71" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="118">
-        <v>77</v>
-      </c>
-      <c r="B80" s="100" t="s">
-        <v>51</v>
-      </c>
-      <c r="C80" s="19"/>
-      <c r="E80" s="14"/>
-    </row>
-    <row r="81" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="118">
-        <v>78</v>
-      </c>
-      <c r="B81" s="100" t="s">
-        <v>52</v>
-      </c>
-      <c r="C81" s="27"/>
-      <c r="E81" s="12"/>
-    </row>
-    <row r="82" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="118">
-        <v>79</v>
-      </c>
-      <c r="B82" s="104" t="s">
-        <v>53</v>
-      </c>
-      <c r="C82" s="47"/>
-      <c r="E82" s="12"/>
-    </row>
-    <row r="83" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="118">
-        <v>80</v>
-      </c>
-      <c r="B83" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="C83" s="62"/>
-      <c r="E83" s="12"/>
-    </row>
-    <row r="84" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="118">
-        <v>81</v>
-      </c>
-      <c r="B84" s="99" t="s">
-        <v>55</v>
-      </c>
-      <c r="C84" s="74"/>
-      <c r="E84" s="12"/>
-    </row>
-    <row r="85" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="118">
-        <v>82</v>
-      </c>
-      <c r="B85" s="100" t="s">
-        <v>56</v>
-      </c>
-      <c r="C85" s="24"/>
-    </row>
-    <row r="86" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="118">
-        <v>83</v>
-      </c>
-      <c r="B86" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="C86" s="35"/>
-      <c r="E86" s="12"/>
-    </row>
-    <row r="87" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="118">
-        <v>84</v>
-      </c>
-      <c r="B87" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C87" s="35"/>
-      <c r="E87" s="12"/>
-    </row>
-    <row r="88" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="118">
-        <v>85</v>
-      </c>
-      <c r="B88" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C88" s="35"/>
-      <c r="E88" s="12"/>
-    </row>
-    <row r="89" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="118">
-        <v>86</v>
-      </c>
-      <c r="B89" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C89" s="35"/>
-      <c r="E89" s="12"/>
-    </row>
-    <row r="90" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="118">
-        <v>87</v>
-      </c>
-      <c r="B90" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C90" s="35"/>
-    </row>
-    <row r="91" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="118">
-        <v>88</v>
-      </c>
-      <c r="B91" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C91" s="35"/>
-    </row>
-    <row r="92" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="118">
-        <v>89</v>
-      </c>
-      <c r="B92" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C92" s="35"/>
-    </row>
-    <row r="93" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="118">
-        <v>90</v>
-      </c>
-      <c r="B93" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C93" s="35"/>
-    </row>
-    <row r="94" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="118">
-        <v>91</v>
-      </c>
-      <c r="B94" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C94" s="35"/>
-    </row>
-    <row r="95" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="118">
-        <v>92</v>
-      </c>
-      <c r="B95" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C95" s="35"/>
-    </row>
-    <row r="96" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="118">
-        <v>93</v>
-      </c>
-      <c r="B96" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C96" s="95"/>
-    </row>
-    <row r="97" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="118">
-        <v>94</v>
-      </c>
-      <c r="B97" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C97" s="35"/>
-    </row>
-    <row r="98" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="118">
-        <v>95</v>
-      </c>
-      <c r="B98" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="C98" s="35"/>
-    </row>
-    <row r="99" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A99" s="118">
-        <v>96</v>
-      </c>
-      <c r="B99" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C99" s="41"/>
-    </row>
-    <row r="100" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="118">
-        <v>97</v>
-      </c>
-      <c r="B100" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C100" s="41"/>
-      <c r="D100" s="15"/>
-    </row>
-    <row r="101" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="118">
-        <v>98</v>
-      </c>
-      <c r="B101" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="C101" s="41"/>
-      <c r="D101" s="15"/>
-    </row>
-    <row r="102" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="118">
-        <v>99</v>
-      </c>
-      <c r="B102" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C102" s="36"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="37" t="s">
+      <c r="B102" s="36"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="C103" s="25" t="s">
+      <c r="B103" s="25" t="s">
         <v>196</v>
       </c>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="C9:C11 C50:C57 C13:C16 C19 C65:C66 C69:C70 C21 C23:C48 C63 C61 C84" name="Диапазон2"/>
-    <protectedRange sqref="C3:C6" name="Диапазон1"/>
-    <protectedRange sqref="C49" name="Диапазон2_1"/>
-    <protectedRange sqref="C12" name="Диапазон2_2"/>
-    <protectedRange sqref="C71:C72 C77:C79 C81:C83 C86:C102" name="Диапазон2_5"/>
+    <protectedRange sqref="B9:B11 B50:B57 B13:B16 B19 B65:B66 B69:B70 B21 B23:B48 B63 B61 B84" name="Диапазон2"/>
+    <protectedRange sqref="B3:B6" name="Диапазон1"/>
+    <protectedRange sqref="B49" name="Диапазон2_1"/>
+    <protectedRange sqref="B12" name="Диапазон2_2"/>
+    <protectedRange sqref="B71:B72 B77:B79 B81:B83 B86:B102" name="Диапазон2_5"/>
   </protectedRanges>
   <mergeCells count="2">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <dataValidations count="22">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B110:B115" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A110:A115" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"кашель сухой, кашель влажный, ринит, диарея, одышка, потеря обоняния, другие симптомы,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C38" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Да (такси), Да (маршрутные автобусы), Да (такси, маршрутные автобусы), Нет, Нет, личный транспорт"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C100" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B100" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"1 подъезд, 2 подъезд, 3 подъезд, 4 подъезд, 5 подъезд, 6 подъезд, 7 подъезд, 8 подъезд, 9 подъезд, 10 подъезд, "</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C101" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B101" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"1 этаж, 2  этаж, 3  этаж, 4  этаж, 5  этаж, 6  этаж, 7  этаж, 8 этаж, 9  этаж, 10  этаж, 11  этаж, 12  этаж, 13  этаж, 14 этаж, 15 этаж, 16 этаж,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C99" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B99" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"Каменный благоустроенный дом, Деревянный благоустроенный дом, Частный дом,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C49" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B49" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Обследование, Контакт, Самообращение, Скриннинг, ОРВИ, Пневмония, Госпитализация"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C53" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B53" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
         <mc:Choice Requires="x12ac">
           <x12ac:list xml:space="preserve"> Центр СПИД, ФБУЗ «ЦГ и Э в РС(Я)», ГАУ РС (Я) МЦ г. Якутска, ГАУ РС (Я) РКБ №3, ГБУ РС (Я) ЯРКБ, ГБУ РС (Я) ЯРОД, ГАУ РС (Я) ЯГБ №3, Клиника СВФУ, НПЦ Фтизиатрия, ГАУ РС(Я) РБ№1-НЦМ," ГБУ РС(Я) ""ЯГБ №2"""," ООО ""Центромед""", Поликлиника №1</x12ac:list>
@@ -3607,56 +3306,56 @@
         </mc:Fallback>
       </mc:AlternateContent>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C56 C34:C36 C45:C47 C71 C77:C79" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56 B34:B36 B45:B47 B71 B77:B79" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"да, нет"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C61 C63" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61 B63" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"Амбулаторно-поликлиническая сеть, Скорая помощь, Стационар неинфекционного профиля, Стационар инфекционного профиля, Прочее"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C57" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B57" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>"Нормальная 36,9, Субфебрильная 37-37,9, Фебрильная 38-38,9, Гипертермия 39 и более, Нет данных"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C69" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B69" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>"Нет, Нет данных, Заболевания органов дыхания, Заболевания сердечно-сосудистой системы, Патология эндокринной системы, Онкологическая патология, Другое"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C39" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>"Нет, Ежедневно, Не более 2-3 раз,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C40:C43" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40:B43" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>"Нет, Однократно, Несколько раз,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C44" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>"Нет, Нахождение в стационаре до 7 дней, Находение в стационаре более 7 дней,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C32" xr:uid="{00000000-0002-0000-0000-00000E000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32" xr:uid="{00000000-0002-0000-0000-00000E000000}">
       <formula1>INDIRECT("ТипСтруктурногоПодразделения")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{00000000-0002-0000-0000-00000F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14" xr:uid="{00000000-0002-0000-0000-00000F000000}">
       <formula1>INDIRECT("УровеньХЦ")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{00000000-0002-0000-0000-000010000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0000-000010000000}">
       <formula1>INDIRECT("СписокРайонов")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{00000000-0002-0000-0000-000011000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19" xr:uid="{00000000-0002-0000-0000-000011000000}">
       <formula1>"Госпитализация, Амбулаторное"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{00000000-0002-0000-0000-000012000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16" xr:uid="{00000000-0002-0000-0000-000012000000}">
       <formula1>"Бессимптомное течение, Легкой степени тяжести, Средней степени тяжести, Тяжелой степени тяжести,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000013000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12" xr:uid="{00000000-0002-0000-0000-000013000000}">
       <formula1>"Мужской, Женский,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000014000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13" xr:uid="{00000000-0002-0000-0000-000014000000}">
       <formula1>INDIRECT("Таблица10[Группа лиц]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33" xr:uid="{00000000-0002-0000-0000-000015000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33" xr:uid="{00000000-0002-0000-0000-000015000000}">
       <formula1>"Нет, Постоянно, От случая к случаю, Редко"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.25" bottom="0.26" header="0.17" footer="0.17"/>
   <pageSetup paperSize="9" scale="67" orientation="portrait" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="6" max="102" man="1"/>
+    <brk id="5" max="102" man="1"/>
   </colBreaks>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -4453,39 +4152,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="114" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="115" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="115"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="115" t="s">
+      <c r="A4" s="117" t="s">
         <v>171</v>
       </c>
-      <c r="B4" s="115"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
       <c r="F4" s="66" t="s">
         <v>201</v>
       </c>
@@ -4494,30 +4193,30 @@
       <c r="I4" s="66"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="113" t="s">
+      <c r="A5" s="116" t="s">
         <v>163</v>
       </c>
-      <c r="B5" s="113"/>
-      <c r="C5" s="113"/>
-      <c r="D5" s="113"/>
-      <c r="E5" s="113"/>
-      <c r="F5" s="113"/>
-      <c r="G5" s="113"/>
-      <c r="H5" s="113"/>
-      <c r="I5" s="113"/>
+      <c r="B5" s="116"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="116"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="113" t="s">
+      <c r="A6" s="116" t="s">
         <v>164</v>
       </c>
-      <c r="B6" s="113"/>
-      <c r="C6" s="113"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
+      <c r="B6" s="116"/>
+      <c r="C6" s="116"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="116"/>
+      <c r="G6" s="116"/>
+      <c r="H6" s="116"/>
+      <c r="I6" s="116"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="64" t="s">
@@ -4528,237 +4227,237 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="114" t="s">
+      <c r="A9" s="112" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="114"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
-      <c r="G9" s="114"/>
-      <c r="H9" s="114"/>
-      <c r="I9" s="114"/>
+      <c r="B9" s="112"/>
+      <c r="C9" s="112"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="112"/>
+      <c r="G9" s="112"/>
+      <c r="H9" s="112"/>
+      <c r="I9" s="112"/>
     </row>
     <row r="10" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="114" t="s">
+      <c r="A10" s="112" t="s">
         <v>166</v>
       </c>
-      <c r="B10" s="114"/>
-      <c r="C10" s="114"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="114"/>
-      <c r="F10" s="114"/>
-      <c r="G10" s="114"/>
-      <c r="H10" s="114"/>
-      <c r="I10" s="114"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="112"/>
+      <c r="D10" s="112"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="112"/>
+      <c r="G10" s="112"/>
+      <c r="H10" s="112"/>
+      <c r="I10" s="112"/>
     </row>
     <row r="11" spans="1:9" s="79" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="110" t="s">
+      <c r="A11" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="110"/>
+      <c r="B11" s="113"/>
       <c r="C11" s="78" t="s">
         <v>191</v>
       </c>
-      <c r="D11" s="110" t="s">
+      <c r="D11" s="113" t="s">
         <v>192</v>
       </c>
-      <c r="E11" s="110"/>
+      <c r="E11" s="113"/>
       <c r="F11" s="78" t="s">
         <v>193</v>
       </c>
-      <c r="G11" s="110" t="s">
+      <c r="G11" s="113" t="s">
         <v>194</v>
       </c>
-      <c r="H11" s="110"/>
+      <c r="H11" s="113"/>
       <c r="I11" s="78" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="79" customFormat="1" ht="42.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="116">
+      <c r="A12" s="110">
         <f>Контактные!B3</f>
         <v>0</v>
       </c>
-      <c r="B12" s="117"/>
+      <c r="B12" s="111"/>
       <c r="C12" s="80">
         <f>Контактные!D3</f>
         <v>0</v>
       </c>
-      <c r="D12" s="116">
+      <c r="D12" s="110">
         <f>Контактные!E3</f>
         <v>0</v>
       </c>
-      <c r="E12" s="117"/>
+      <c r="E12" s="111"/>
       <c r="F12" s="81">
         <f>Контактные!F3</f>
         <v>0</v>
       </c>
-      <c r="G12" s="116">
+      <c r="G12" s="110">
         <f>Контактные!G3</f>
         <v>0</v>
       </c>
-      <c r="H12" s="117"/>
+      <c r="H12" s="111"/>
       <c r="I12" s="82">
         <f>Контактные!I3</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="79" customFormat="1" ht="40.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="116">
+      <c r="A13" s="110">
         <f>Контактные!B4</f>
         <v>0</v>
       </c>
-      <c r="B13" s="117"/>
+      <c r="B13" s="111"/>
       <c r="C13" s="80">
         <f>Контактные!D4</f>
         <v>0</v>
       </c>
-      <c r="D13" s="116">
+      <c r="D13" s="110">
         <f>Контактные!E4</f>
         <v>0</v>
       </c>
-      <c r="E13" s="117"/>
+      <c r="E13" s="111"/>
       <c r="F13" s="81">
         <f>Контактные!F4</f>
         <v>0</v>
       </c>
-      <c r="G13" s="116">
+      <c r="G13" s="110">
         <f>Контактные!G4</f>
         <v>0</v>
       </c>
-      <c r="H13" s="117"/>
+      <c r="H13" s="111"/>
       <c r="I13" s="82">
         <f>Контактные!I4</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="79" customFormat="1" ht="41.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="116">
+      <c r="A14" s="110">
         <f>Контактные!B5</f>
         <v>0</v>
       </c>
-      <c r="B14" s="117"/>
+      <c r="B14" s="111"/>
       <c r="C14" s="80">
         <f>Контактные!D5</f>
         <v>0</v>
       </c>
-      <c r="D14" s="116">
+      <c r="D14" s="110">
         <f>Контактные!E5</f>
         <v>0</v>
       </c>
-      <c r="E14" s="117"/>
+      <c r="E14" s="111"/>
       <c r="F14" s="81">
         <f>Контактные!F5</f>
         <v>0</v>
       </c>
-      <c r="G14" s="116">
+      <c r="G14" s="110">
         <f>Контактные!G5</f>
         <v>0</v>
       </c>
-      <c r="H14" s="117"/>
+      <c r="H14" s="111"/>
       <c r="I14" s="82">
         <f>Контактные!I5</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="79" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="116">
+      <c r="A15" s="110">
         <f>Контактные!B6</f>
         <v>0</v>
       </c>
-      <c r="B15" s="117"/>
+      <c r="B15" s="111"/>
       <c r="C15" s="80">
         <f>Контактные!D6</f>
         <v>0</v>
       </c>
-      <c r="D15" s="116">
+      <c r="D15" s="110">
         <f>Контактные!E6</f>
         <v>0</v>
       </c>
-      <c r="E15" s="117"/>
+      <c r="E15" s="111"/>
       <c r="F15" s="81">
         <f>Контактные!F6</f>
         <v>0</v>
       </c>
-      <c r="G15" s="116">
+      <c r="G15" s="110">
         <f>Контактные!G6</f>
         <v>0</v>
       </c>
-      <c r="H15" s="117"/>
+      <c r="H15" s="111"/>
       <c r="I15" s="82">
         <f>Контактные!I6</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="79" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="116">
+      <c r="A16" s="110">
         <f>Контактные!B7</f>
         <v>0</v>
       </c>
-      <c r="B16" s="117"/>
+      <c r="B16" s="111"/>
       <c r="C16" s="80">
         <f>Контактные!D7</f>
         <v>0</v>
       </c>
-      <c r="D16" s="116">
+      <c r="D16" s="110">
         <f>Контактные!E7</f>
         <v>0</v>
       </c>
-      <c r="E16" s="117"/>
+      <c r="E16" s="111"/>
       <c r="F16" s="81">
         <f>Контактные!F7</f>
         <v>0</v>
       </c>
-      <c r="G16" s="116">
+      <c r="G16" s="110">
         <f>Контактные!G7</f>
         <v>0</v>
       </c>
-      <c r="H16" s="117"/>
+      <c r="H16" s="111"/>
       <c r="I16" s="82">
         <f>Контактные!I7</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="114" t="s">
+      <c r="A17" s="112" t="s">
         <v>167</v>
       </c>
-      <c r="B17" s="114"/>
-      <c r="C17" s="114"/>
-      <c r="D17" s="114"/>
-      <c r="E17" s="114"/>
-      <c r="F17" s="114"/>
-      <c r="G17" s="114"/>
-      <c r="H17" s="114"/>
-      <c r="I17" s="114"/>
+      <c r="B17" s="112"/>
+      <c r="C17" s="112"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="112"/>
+      <c r="F17" s="112"/>
+      <c r="G17" s="112"/>
+      <c r="H17" s="112"/>
+      <c r="I17" s="112"/>
     </row>
     <row r="18" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="114" t="s">
+      <c r="A18" s="112" t="s">
         <v>168</v>
       </c>
-      <c r="B18" s="114"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="114"/>
-      <c r="G18" s="114"/>
-      <c r="H18" s="114"/>
-      <c r="I18" s="114"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="112"/>
+      <c r="I18" s="112"/>
     </row>
     <row r="19" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="114" t="s">
+      <c r="A19" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="B19" s="114"/>
-      <c r="C19" s="114"/>
-      <c r="D19" s="114"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="114"/>
-      <c r="G19" s="114"/>
-      <c r="H19" s="114"/>
-      <c r="I19" s="114"/>
+      <c r="B19" s="112"/>
+      <c r="C19" s="112"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="112"/>
+      <c r="F19" s="112"/>
+      <c r="G19" s="112"/>
+      <c r="H19" s="112"/>
+      <c r="I19" s="112"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="91" t="s">
@@ -4802,24 +4501,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A18:I18"/>
-    <mergeCell ref="A19:I19"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
@@ -4830,6 +4511,24 @@
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="98" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>